<commit_message>
1-treeview added; 2-context menu for pivot and project; 3- differentiating relations from types from entities
</commit_message>
<xml_diff>
--- a/TODO-Demo.xlsx
+++ b/TODO-Demo.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SPRINT 2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>1 - Corrigir Paginação (2 h)</t>
   </si>
@@ -91,13 +92,106 @@
   </si>
   <si>
     <t>Implementação do conjunto usando jstree</t>
+  </si>
+  <si>
+    <t>jstree</t>
+  </si>
+  <si>
+    <t>25 min</t>
+  </si>
+  <si>
+    <t>18 - Corrigir Group</t>
+  </si>
+  <si>
+    <t>19 - Corrigir Rank</t>
+  </si>
+  <si>
+    <t>20 - Corrigir Refine</t>
+  </si>
+  <si>
+    <t>21 - Corrigir Map</t>
+  </si>
+  <si>
+    <t>Adicionar Backward Properties</t>
+  </si>
+  <si>
+    <t>Corrigir keyword search</t>
+  </si>
+  <si>
+    <t>Corrigir projeção</t>
+  </si>
+  <si>
+    <t>Implementar Highligths</t>
+  </si>
+  <si>
+    <t>implementar seleção de property paths na interface para pivot</t>
+  </si>
+  <si>
+    <t>implementar seleção de property paths na interface para refine</t>
+  </si>
+  <si>
+    <t>Corrigir testes do framework</t>
+  </si>
+  <si>
+    <t>Implementar a abreviação dos namespaces</t>
+  </si>
+  <si>
+    <t>Diferenciar literais de entidades e de relações</t>
+  </si>
+  <si>
+    <t>Corrigir filtro por palavra chave</t>
+  </si>
+  <si>
+    <t>Implementar seleção de repositórios</t>
+  </si>
+  <si>
+    <t>Implementar findPath no framework</t>
+  </si>
+  <si>
+    <t>Implementar o resultado de paths na view sem aninhamento</t>
+  </si>
+  <si>
+    <t>implementar a exploração da intenção com marcação dos conjuntos de origem envolvidos.</t>
+  </si>
+  <si>
+    <t>Definir as categorias e o style para cada categoria de itens na interface</t>
+  </si>
+  <si>
+    <t>Corrigir a função de Rank</t>
+  </si>
+  <si>
+    <t>Pesquisar framework para visualização em grafo dos conjuntos</t>
+  </si>
+  <si>
+    <t>Implementar a execução das operações a partir dos itens selecionados na interface. O usuário pode escolher se quer aplicar a operação para o elemento corrente ou para todo o conjunto</t>
+  </si>
+  <si>
+    <t>Inserir os conjuntos gerados sempre no início</t>
+  </si>
+  <si>
+    <t>TAREFAS</t>
+  </si>
+  <si>
+    <t>HORAS PREVISTAS</t>
+  </si>
+  <si>
+    <t>HORAS EFETUADAS</t>
+  </si>
+  <si>
+    <t>COMENTÁRIOS</t>
+  </si>
+  <si>
+    <t>Testar a base de publicações mais atual</t>
+  </si>
+  <si>
+    <t>Modificar o conceito da ferramenta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,16 +215,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -138,18 +263,67 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,15 +653,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="73.1640625" customWidth="1"/>
+    <col min="1" max="1" width="118.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" customWidth="1"/>
@@ -508,34 +682,37 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="1" customFormat="1">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:4" s="1" customFormat="1">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
     </row>
@@ -548,11 +725,11 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>8</v>
@@ -610,11 +787,17 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -642,28 +825,53 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="1" customFormat="1">
+      <c r="A19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="2" customFormat="1">
+      <c r="A20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="2" customFormat="1">
+      <c r="A21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="2" customFormat="1">
+      <c r="A22" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" s="2" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>21</v>
       </c>
-      <c r="B20">
-        <f>SUM(B2:B19)</f>
-        <v>62</v>
+      <c r="B25">
+        <f>SUM(B2:B24)</f>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -675,4 +883,306 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="83.83203125" style="5" customWidth="1"/>
+    <col min="2" max="3" width="25.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.1640625" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="3">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="3">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="6">
+        <f>SUM(B2:B29)</f>
+        <v>52.5</v>
+      </c>
+      <c r="C30" s="6">
+        <f>SUM(C2:C29)</f>
+        <v>0</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of bootstrap for layout; initial implementation of graph view.
</commit_message>
<xml_diff>
--- a/TODO-Demo.xlsx
+++ b/TODO-Demo.xlsx
@@ -9,7 +9,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="SPRINT 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprint 3" sheetId="4" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SPRINT 2'!$A$1:$E$26</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
     <t>1 - Corrigir Paginação (2 h)</t>
   </si>
@@ -185,6 +189,45 @@
   </si>
   <si>
     <t>Modificar o conceito da ferramenta</t>
+  </si>
+  <si>
+    <t>Implementar keyword search por índices</t>
+  </si>
+  <si>
+    <t>Implementar seleção de múltiplos itens na interface</t>
+  </si>
+  <si>
+    <t>Horas Restantes</t>
+  </si>
+  <si>
+    <t>Union não estava implementada; correção na operação de join; bug em variáveis js</t>
+  </si>
+  <si>
+    <t>Implementar pivot para todas as relações do conjunto</t>
+  </si>
+  <si>
+    <t>Problemas na modificação dos ícones pela jtree; adição de fonte do bootstrap</t>
+  </si>
+  <si>
+    <t>Modificar seleção de property paths para carregar relações aninhadas ao abrir ao invés de no momento da seleção</t>
+  </si>
+  <si>
+    <t>Refatorar framework para garantir uma melhor separação entre interface e execução de operações</t>
+  </si>
+  <si>
+    <t>Implementar a apresentação de backward properties</t>
+  </si>
+  <si>
+    <t>Corrigir o property path pivot para admitir caminhos com propriedades inversas</t>
+  </si>
+  <si>
+    <t>Corrigir interface para o property path pivot para admitir caminhos com propriedades inversas</t>
+  </si>
+  <si>
+    <t>desabilitar checkbox de relações</t>
+  </si>
+  <si>
+    <t>Corrigir operação Refine para diferenciar itens de literais</t>
   </si>
 </sst>
 </file>
@@ -229,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +294,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -279,7 +328,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -297,8 +346,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -306,8 +359,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -316,6 +375,8 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -324,6 +385,8 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -887,21 +950,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="83.83203125" style="5" customWidth="1"/>
-    <col min="2" max="3" width="25.6640625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.1640625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="5"/>
+    <col min="2" max="4" width="25.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="31.1640625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
@@ -909,276 +972,644 @@
         <v>50</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" s="8" customFormat="1">
+      <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="3" t="s">
+      <c r="C2" s="7">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1">
+      <c r="A3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="7">
         <v>0.5</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="3" t="s">
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" s="8" customFormat="1">
+      <c r="A4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="7">
         <v>0.5</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="B6" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="3" t="s">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" s="8" customFormat="1">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7">
+        <v>8</v>
+      </c>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="3" t="s">
+      <c r="C8" s="3">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B9" s="3">
         <v>6</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="3" t="s">
+      <c r="C9" s="3">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B10" s="3">
         <v>0.5</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" s="8" customFormat="1">
+      <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B11" s="7">
         <v>1</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="8" customFormat="1">
+      <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="7">
         <v>0.5</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B12" s="3">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3">
+        <v>4</v>
+      </c>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>4</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="3">
-        <v>2</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="3" t="s">
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>6</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="3" t="s">
+      <c r="C16" s="3">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="3">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="C18" s="3">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1">
+      <c r="A19" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="3">
-        <v>2</v>
-      </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="7">
+        <v>2</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <v>8</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="8" customFormat="1">
+      <c r="A20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="7">
         <v>0.5</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
+      <c r="C20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="3">
-        <v>2</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="3">
-        <v>2</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
       <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3">
+        <v>8</v>
+      </c>
+      <c r="C23" s="3">
+        <v>8</v>
+      </c>
       <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="3"/>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" s="8" customFormat="1">
+      <c r="A24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E24" s="7"/>
+    </row>
+    <row r="25" spans="1:5" s="8" customFormat="1">
+      <c r="A25" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="7">
+        <v>24</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>24</v>
+      </c>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" s="8" customFormat="1">
+      <c r="A26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="7">
+        <v>2</v>
+      </c>
+      <c r="C26" s="7">
+        <v>2</v>
+      </c>
+      <c r="D26" s="7">
+        <v>2</v>
+      </c>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="6" t="s">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="6">
-        <f>SUM(B2:B29)</f>
-        <v>52.5</v>
-      </c>
-      <c r="C30" s="6">
-        <f>SUM(C2:C29)</f>
-        <v>0</v>
-      </c>
-      <c r="D30" s="3"/>
+      <c r="B31" s="6">
+        <f>SUM(B2:B30)</f>
+        <v>88</v>
+      </c>
+      <c r="C31" s="6">
+        <f>SUM(C2:C30)</f>
+        <v>57.5</v>
+      </c>
+      <c r="D31" s="6">
+        <f>SUM(D2:D30)</f>
+        <v>50</v>
+      </c>
+      <c r="E31" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:E26"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="57" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18">
+      <c r="A2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" ht="18">
+      <c r="A4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="D4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+    </row>
+    <row r="8" spans="1:5" ht="18">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="1:5" ht="18">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="1:5" ht="18">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+    </row>
+    <row r="11" spans="1:5" ht="18">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" ht="18">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" ht="18">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" ht="18">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" ht="18">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" ht="18">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" ht="18">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" ht="18">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9">
+        <v>8</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" ht="18">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="18">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>